<commit_message>
new excel template and changed min-max value interface
</commit_message>
<xml_diff>
--- a/Example for Login and Design/excel/start_default.xlsx
+++ b/Example for Login and Design/excel/start_default.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/PHPExcel-develop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/DVA313-Solar-Energy/Example for Login and Design/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="60" yWindow="920" windowWidth="15420" windowHeight="15220" tabRatio="500"/>
+    <workbookView xWindow="400" yWindow="920" windowWidth="15420" windowHeight="15220" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Indata och resultat privatperso" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="160">
   <si>
     <t>Anläggning</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Anläggningens effekt</t>
   </si>
   <si>
-    <t>Modylyta</t>
-  </si>
-  <si>
     <t>Säkringsstorlek i anslutningspunkten</t>
   </si>
   <si>
@@ -140,9 +137,6 @@
     <t>Cellerna ändrar automatiskt färg mellan grön och röd beroende på om värdena är positiva eller negativa.</t>
   </si>
   <si>
-    <t>Ekonomisk livslängd (N)</t>
-  </si>
-  <si>
     <t>Ekonomisk livslängd</t>
   </si>
   <si>
@@ -209,9 +203,6 @@
     <t>Intäkter</t>
   </si>
   <si>
-    <t xml:space="preserve">Värden anges som uppskattat medel av nuvärden under anläggningens livslängd. En svårighet är att uppskatta värdena under så lång tid framåt som solcellssystemets livslängd. </t>
-  </si>
-  <si>
     <t>Andel egenanvänd el</t>
   </si>
   <si>
@@ -248,9 +239,6 @@
     <t xml:space="preserve">Endast heltal år beräknas för återbetalningstiden. </t>
   </si>
   <si>
-    <t xml:space="preserve">De faktorer som har störst inverkan på lönsamheten är investeringskostnad, kalkylränta, andel egenanvänd el och värdet av egenanvänd respektive såld el, där speciellt skattereduktionen har en stor betydelse. </t>
-  </si>
-  <si>
     <t>Utan ROT-avdrag och investeringsstöd, med eventuell skattereduktion</t>
   </si>
   <si>
@@ -281,9 +269,6 @@
     <t>%</t>
   </si>
   <si>
-    <t>Kalkylränta (R)</t>
-  </si>
-  <si>
     <t>kr/kW</t>
   </si>
   <si>
@@ -519,6 +504,12 @@
   </si>
   <si>
     <t>Man kan få skattereduktion för högst 30 000 kWh/år, eller högst för så mycket el man köper under ett år, per person eller anslutningspunkt enligt Inkomstskattelag (1999:1229). Vid en skattereduktion på 60 öre/kWh blir taket därmed 18 000 kr per år. Här antas att överskottet är mindre den egna elanvändningen och att skattereduktion därmed kan utnyttjas för hela överskottet upp till takbeloppet som mest.</t>
+  </si>
+  <si>
+    <t>Modulyta</t>
+  </si>
+  <si>
+    <t>Värden anges som uppskattat medel av nuvärden under anläggningens livslängd.</t>
   </si>
 </sst>
 </file>
@@ -863,7 +854,7 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -878,22 +869,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -912,57 +903,57 @@
         <v>4</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D20">
         <v>16</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>25</v>
@@ -971,23 +962,23 @@
         <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D28">
         <v>25</v>
@@ -996,23 +987,23 @@
         <v>30</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>19000</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D32">
         <v>9000</v>
@@ -1021,18 +1012,18 @@
         <v>25000</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D33">
         <v>20</v>
@@ -1041,52 +1032,52 @@
         <v>35</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>2000</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1095,119 +1086,119 @@
         <v>10000</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>900</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D53">
         <v>700</v>
@@ -1216,50 +1207,50 @@
         <v>1200</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>50</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1268,18 +1259,18 @@
         <v>100</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>1.4</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D61">
         <v>0.5</v>
@@ -1288,18 +1279,18 @@
         <v>1.5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>0.5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1308,18 +1299,18 @@
         <v>1.5</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>0.05</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D63">
         <v>0.02</v>
@@ -1328,18 +1319,18 @@
         <v>0.06</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>0.13</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D64">
         <v>0.1</v>
@@ -1348,18 +1339,18 @@
         <v>0.2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>50</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -1368,18 +1359,18 @@
         <v>100</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -1388,18 +1379,18 @@
         <v>23</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -1408,167 +1399,164 @@
         <v>0.02</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>15</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F79" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1580,8 +1568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1596,22 +1584,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1630,57 +1618,57 @@
         <v>100</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>2</v>
+        <v>158</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20">
         <v>150</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D20">
         <v>16</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B24">
         <v>30</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>25</v>
@@ -1689,23 +1677,23 @@
         <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28">
         <v>5</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -1714,23 +1702,23 @@
         <v>10</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>11000</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D32">
         <v>9000</v>
@@ -1739,18 +1727,18 @@
         <v>25000</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33">
         <v>30</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D33">
         <v>20</v>
@@ -1759,52 +1747,52 @@
         <v>35</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35">
         <v>10000</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B37">
         <v>10000</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1813,119 +1801,119 @@
         <v>10000</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B53">
         <v>950</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D53">
         <v>700</v>
@@ -1934,50 +1922,50 @@
         <v>1200</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>80</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1986,18 +1974,18 @@
         <v>100</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="224" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B61">
         <v>1.1000000000000001</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D61">
         <v>0.5</v>
@@ -2006,18 +1994,18 @@
         <v>1.5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B62">
         <v>0.5</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -2026,18 +2014,18 @@
         <v>1.5</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B63">
         <v>0.05</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D63">
         <v>0.02</v>
@@ -2046,18 +2034,18 @@
         <v>0.06</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B64">
         <v>0.13</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D64">
         <v>0.1</v>
@@ -2066,18 +2054,18 @@
         <v>0.2</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B65">
         <v>100</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2086,18 +2074,18 @@
         <v>100</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B66">
         <v>0</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2106,18 +2094,18 @@
         <v>23</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B67">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -2126,167 +2114,164 @@
         <v>0.02</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B68">
         <v>15</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D68">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="112" x14ac:dyDescent="0.2">
-      <c r="A79" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F79" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2298,8 +2283,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E69" sqref="E69"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2314,22 +2299,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2342,13 +2327,13 @@
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B12">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -2357,23 +2342,23 @@
         <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>1200000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D16">
         <v>1200000</v>
@@ -2382,18 +2367,18 @@
         <v>1200000</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -2402,18 +2387,18 @@
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18">
         <v>50000</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D18">
         <v>50000</v>
@@ -2422,46 +2407,46 @@
         <v>100000</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -2473,18 +2458,18 @@
         <v>2</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B24">
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -2493,15 +2478,15 @@
         <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2510,113 +2495,113 @@
         <v>3000</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B32">
         <v>0</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2624,201 +2609,201 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -2826,18 +2811,18 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B56">
         <v>0.3</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D56">
         <v>0.1</v>
@@ -2846,23 +2831,23 @@
         <v>0.5</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B60">
         <v>99.9</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D60">
         <v>98</v>
@@ -2871,23 +2856,23 @@
         <v>100</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B64">
         <v>15</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -2896,18 +2881,18 @@
         <v>15</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B65">
         <v>0.6</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -2916,18 +2901,18 @@
         <v>0.6</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B66">
         <v>18000</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -2936,7 +2921,7 @@
         <v>18000</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2964,22 +2949,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -2992,13 +2977,13 @@
     </row>
     <row r="12" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B12">
         <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -3007,23 +2992,23 @@
         <v>21</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B16">
         <v>1200000</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D16">
         <v>1200000</v>
@@ -3032,18 +3017,18 @@
         <v>1200000</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -3052,18 +3037,18 @@
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B18">
         <v>50000</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D18">
         <v>50000</v>
@@ -3072,46 +3057,46 @@
         <v>100000</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B21">
         <v>0</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3123,18 +3108,18 @@
         <v>2</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B24">
         <v>15</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D24">
         <v>10</v>
@@ -3143,15 +3128,15 @@
         <v>30</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -3160,113 +3145,113 @@
         <v>3000</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B30">
         <v>2000</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B32">
         <v>2000</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B33">
         <v>0</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B34">
         <v>1000</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -3274,201 +3259,201 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B41">
         <v>0</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B45">
         <v>5000</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -3476,18 +3461,18 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B56">
         <v>0.3</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D56">
         <v>0.1</v>
@@ -3496,23 +3481,23 @@
         <v>0.5</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B60">
         <v>99.9</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D60">
         <v>98</v>
@@ -3521,23 +3506,23 @@
         <v>100</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B64">
         <v>15</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -3546,18 +3531,18 @@
         <v>15</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B65">
         <v>0.6</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -3566,18 +3551,18 @@
         <v>0.6</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B66">
         <v>18000</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -3586,7 +3571,7 @@
         <v>18000</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>